<commit_message>
Finished writing all the code.
</commit_message>
<xml_diff>
--- a/Test data/TC04_ReserveVaccine.xlsx
+++ b/Test data/TC04_ReserveVaccine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Project\Test data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D994E12C-A2A0-44B3-9471-C78EB6F48310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A92AD5-64FA-4DB4-BAF1-BFD43E078B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -525,7 +525,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
@@ -581,7 +581,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>8</v>
@@ -608,7 +608,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>8</v>
@@ -689,7 +689,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>8</v>
@@ -718,7 +718,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>8</v>

</xml_diff>